<commit_message>
Conceptos IVAs Almacenes y Tipos de Documento
</commit_message>
<xml_diff>
--- a/MiAppComercial.xlsx
+++ b/MiAppComercial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos\MiAppComercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD9F018-8644-4D3F-A32C-CACBD8C2D1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A69BEC6-1B93-4123-8AD8-6A91D7D6449C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2304E8A-2790-4DC1-9361-D98A59767F40}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Login</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Ventas con filtro</t>
+  </si>
+  <si>
+    <t>Tipos de documento</t>
   </si>
 </sst>
 </file>
@@ -570,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37124253-E01A-4385-92A0-6B1F6853F919}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5546875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -617,7 +620,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -625,7 +628,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -633,7 +636,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -641,7 +644,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -649,8 +652,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
+      <c r="A9" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>34</v>
@@ -658,7 +661,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>35</v>
@@ -666,7 +669,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>36</v>
@@ -674,7 +677,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>37</v>
@@ -682,7 +685,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>21</v>
@@ -690,7 +693,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>45</v>
@@ -698,7 +701,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>30</v>
@@ -706,7 +709,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>31</v>
@@ -714,7 +717,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>32</v>
@@ -722,7 +725,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>38</v>
@@ -730,7 +733,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>40</v>
@@ -738,7 +741,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>39</v>
@@ -746,7 +749,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>22</v>
@@ -754,7 +757,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>23</v>
@@ -762,7 +765,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>7</v>
@@ -770,10 +773,15 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambio Usuario y Cambio Clave
</commit_message>
<xml_diff>
--- a/MiAppComercial.xlsx
+++ b/MiAppComercial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos\MiAppComercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D05660-5A21-4ADF-A49D-F019103FDD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AEA250-BC01-4473-99D6-683F29B940C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2304E8A-2790-4DC1-9361-D98A59767F40}"/>
   </bookViews>
@@ -576,7 +576,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A17" sqref="A17:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5546875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -708,7 +708,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -716,7 +716,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -724,7 +724,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="3" t="s">

</xml_diff>

<commit_message>
Ajustes de Inventario Ok
</commit_message>
<xml_diff>
--- a/MiAppComercial.xlsx
+++ b/MiAppComercial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos\MiAppComercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6767FF0-E41B-4875-83AD-AE14BAD74CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45301611-80E4-4FA5-A546-D6AE0B3D3D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2304E8A-2790-4DC1-9361-D98A59767F40}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Login</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>Devolución Proveedores nueva</t>
+  </si>
+  <si>
+    <t>Falta poder imprimir el listado</t>
+  </si>
+  <si>
+    <t>Inventarios con filtros</t>
   </si>
 </sst>
 </file>
@@ -600,7 +606,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5546875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -684,8 +690,11 @@
       <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -717,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -725,7 +734,7 @@
         <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -733,7 +742,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -741,7 +750,7 @@
         <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -749,7 +758,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -757,7 +766,7 @@
         <v>20</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -768,7 +777,7 @@
         <v>45</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -776,7 +785,7 @@
         <v>24</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -787,7 +796,7 @@
         <v>45</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -795,7 +804,7 @@
         <v>43</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -806,7 +815,7 @@
         <v>46</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -817,7 +826,7 @@
         <v>47</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -826,6 +835,9 @@
       </c>
       <c r="B25" s="1" t="s">
         <v>48</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Consulta Inventarios a medio hacer
</commit_message>
<xml_diff>
--- a/MiAppComercial.xlsx
+++ b/MiAppComercial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos\MiAppComercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C9A1DC-D616-4E9E-80BB-25A7450A0652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204FAB1C-0C3D-4985-A312-EC4EDF0970D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2304E8A-2790-4DC1-9361-D98A59767F40}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
   <si>
     <t>Login</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Ver un Inventario</t>
+  </si>
+  <si>
+    <t>Falta el Detalle</t>
   </si>
 </sst>
 </file>
@@ -276,7 +279,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -645,7 +648,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5546875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -662,7 +665,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -686,7 +689,7 @@
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -734,7 +737,7 @@
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -839,8 +842,11 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>56</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>26</v>
@@ -882,7 +888,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D27" s="3" t="s">

</xml_diff>

<commit_message>
Consulta de una Compra y de una Venta
</commit_message>
<xml_diff>
--- a/MiAppComercial.xlsx
+++ b/MiAppComercial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos\MiAppComercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB18250-1ED9-40B0-A583-5F6C54CC4224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2F5E30-AB8A-4381-8CEC-F6C3B1490D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2304E8A-2790-4DC1-9361-D98A59767F40}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
   <si>
     <t>Login</t>
   </si>
@@ -225,16 +225,13 @@
   </si>
   <si>
     <t>Falta el Detalle</t>
-  </si>
-  <si>
-    <t>A medio hacer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,13 +258,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -290,7 +280,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -336,13 +326,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -662,7 +649,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5546875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -687,7 +674,7 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -711,7 +698,7 @@
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>59</v>
       </c>
     </row>
@@ -735,7 +722,7 @@
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>60</v>
       </c>
     </row>
@@ -759,7 +746,7 @@
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>61</v>
       </c>
     </row>
@@ -816,21 +803,18 @@
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
@@ -860,7 +844,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -906,7 +890,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D27" s="3" t="s">

</xml_diff>

<commit_message>
Consulta Una Devolución a Proveedor
</commit_message>
<xml_diff>
--- a/MiAppComercial.xlsx
+++ b/MiAppComercial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos\MiAppComercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A580403-222C-4DAA-9206-57BD899A0541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489E637F-C700-4D46-97BD-496CC8FE3E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2304E8A-2790-4DC1-9361-D98A59767F40}"/>
   </bookViews>
@@ -646,7 +646,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5546875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -719,7 +719,7 @@
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="2" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Consulta una Devolución de Cliente
</commit_message>
<xml_diff>
--- a/MiAppComercial.xlsx
+++ b/MiAppComercial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos\MiAppComercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489E637F-C700-4D46-97BD-496CC8FE3E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C29CACB-1CE2-4272-93F1-EBD55DC8083A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2304E8A-2790-4DC1-9361-D98A59767F40}"/>
   </bookViews>
@@ -646,7 +646,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5546875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -671,7 +671,7 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="2" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Parcial En todos los Ver un poder cambiar el ID para buscar otro
</commit_message>
<xml_diff>
--- a/MiAppComercial.xlsx
+++ b/MiAppComercial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos\MiAppComercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6C8909-9ABA-4C8D-8F2E-D90FF4F46F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1959135E-269B-465B-A512-1FAEDADF8582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2304E8A-2790-4DC1-9361-D98A59767F40}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
   <si>
     <t>Login</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Ver un Inventario</t>
+  </si>
+  <si>
+    <t>En todos los "Ver un" poder cambiar el ID para buscar otro</t>
   </si>
 </sst>
 </file>
@@ -277,7 +280,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -643,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37124253-E01A-4385-92A0-6B1F6853F919}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5546875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -671,7 +674,7 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -695,7 +698,7 @@
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
         <v>59</v>
       </c>
     </row>
@@ -719,7 +722,7 @@
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="6" t="s">
         <v>60</v>
       </c>
     </row>
@@ -743,7 +746,7 @@
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="6" t="s">
         <v>61</v>
       </c>
     </row>
@@ -841,7 +844,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="6" t="s">
         <v>56</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -884,7 +887,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -916,6 +919,11 @@
       </c>
       <c r="D30" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D32" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Consultas Ver un completas
</commit_message>
<xml_diff>
--- a/MiAppComercial.xlsx
+++ b/MiAppComercial.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos\MiAppComercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1959135E-269B-465B-A512-1FAEDADF8582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE409B9-7B3D-491A-AACC-39004555A6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2304E8A-2790-4DC1-9361-D98A59767F40}"/>
   </bookViews>
@@ -312,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -330,6 +330,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -649,7 +652,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5546875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -844,7 +847,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -887,7 +890,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -922,7 +925,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="7" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correcion error al hacer clic en datagridview
</commit_message>
<xml_diff>
--- a/MiAppComercial.xlsx
+++ b/MiAppComercial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos\MiAppComercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D607376-A16C-432B-B1C5-ED46FDFA9121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C8285F-6637-4AAC-B232-B6D657FA0A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2304E8A-2790-4DC1-9361-D98A59767F40}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Login</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Tipos de documento</t>
   </si>
   <si>
-    <t>Da error al hacer clic en el datagridview</t>
-  </si>
-  <si>
     <t>Verificarlo bien con todos los movimientos</t>
   </si>
   <si>
@@ -222,6 +219,9 @@
   </si>
   <si>
     <t>En todos los "Ver un" poder cambiar el ID para buscar otro</t>
+  </si>
+  <si>
+    <t>Cambio de Precios Costos y Utilidades</t>
   </si>
 </sst>
 </file>
@@ -634,275 +634,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37124253-E01A-4385-92A0-6B1F6853F919}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:E15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5546875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.5546875" style="1"/>
-    <col min="4" max="4" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="3.5546875" style="1"/>
+    <col min="3" max="3" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="3.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C31" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="3" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C32" s="3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D31" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>